<commit_message>
adding new html pages for song display
</commit_message>
<xml_diff>
--- a/Assignments/Brea/Capstone/Brea Capstone Database Proposal.xlsx
+++ b/Assignments/Brea/Capstone/Brea Capstone Database Proposal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mura6568/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mura6568/Desktop/Coding/class_mudpuppy/Assignments/Brea/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C641293C-92AC-4446-91FF-0041AF7BE313}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607CCF25-819C-0E4E-8DD0-043AE889C03F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="460" windowWidth="23860" windowHeight="17540" activeTab="2" xr2:uid="{2F071B6E-C72B-CB4F-8EC4-3FEEAC056547}"/>
+    <workbookView xWindow="18800" yWindow="0" windowWidth="10000" windowHeight="18000" activeTab="2" xr2:uid="{2F071B6E-C72B-CB4F-8EC4-3FEEAC056547}"/>
   </bookViews>
   <sheets>
     <sheet name="Song Input" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Wikipedia Link</t>
   </si>
   <si>
-    <t>(Links to Other Tables)</t>
-  </si>
-  <si>
     <t>Tempo</t>
   </si>
   <si>
@@ -222,13 +219,106 @@
   </si>
   <si>
     <t>Text box</t>
+  </si>
+  <si>
+    <t>Giving Up</t>
+  </si>
+  <si>
+    <t>Ingrid Michaelson</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/58jSGbni8xnVEi9xjDaqtK?si=oAEG5h9aRc26TBeDBBj3Ww</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Ingrid_Michaelson</t>
+  </si>
+  <si>
+    <t>https://tabs.ultimate-guitar.com/tab/ingrid-michaelson/giving-up-chords-1052454</t>
+  </si>
+  <si>
+    <t>Fast Car</t>
+  </si>
+  <si>
+    <t>Tracy Chapman</t>
+  </si>
+  <si>
+    <t>https://tabs.ultimate-guitar.com/tab/tracy-chapman/fast-car-chords-1044807</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Tracy_Chapman</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/2M9ro2krNb7nr7HSprkEgo?si=uzqQ15UXSr-B-dtSo_O5OA</t>
+  </si>
+  <si>
+    <t>Savage Remix</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Megan_Thee_Stallion</t>
+  </si>
+  <si>
+    <t>https://tabs.ultimate-guitar.com/tab/megan-thee-stallion/savage-chords-3102686</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/5v4GgrXPMghOnBBLmveLac?si=C93kHHIXRiyRP2tLGSh8Dg</t>
+  </si>
+  <si>
+    <t>Do Not Disturb</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/2KvHC9z14GSl4YpkNMX384?si=2-BC9hnMRQGMf-g6FuuwCw</t>
+  </si>
+  <si>
+    <t>https://tabs.ultimate-guitar.com/tab/drake/do-not-disturb-chords-1969991</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/More_Life</t>
+  </si>
+  <si>
+    <t>If It Be Your Will</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/65sKEPMT59DU07NXTGAEj4?si=42KMUCzVQLGC5L7RWcMWRA</t>
+  </si>
+  <si>
+    <t>Cover?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Loud Places</t>
+  </si>
+  <si>
+    <t>Jamie xx; Romy</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/2JQm8NNpFkwvhuKH3yhuC9?si=9PPJhDSPT2mk1_5UwKB8ow</t>
+  </si>
+  <si>
+    <t>Megan Thee Stallion; Beyoncé</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Loud_Places</t>
+  </si>
+  <si>
+    <t>https://tabs.ultimate-guitar.com/tab/jamie-xx/loud-places-chords-1742525</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +339,14 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,17 +365,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -590,22 +691,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F268A2C-38E7-8245-A767-5B7EF2AD366D}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
-    <col min="2" max="6" width="19.83203125" style="1"/>
+    <col min="2" max="4" width="19.83203125" style="1"/>
+    <col min="5" max="5" width="47.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" style="1"/>
     <col min="7" max="7" width="22.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="34" style="1" customWidth="1"/>
     <col min="9" max="16384" width="19.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,23 +728,148 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1988</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2006</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{453F77EE-5B78-5041-A342-51ACCAB31984}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{DD12FA3F-BF66-E94D-80C5-E2353FD7FE04}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{E4D18AAA-F9F1-1D45-A51A-3D476C347206}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{2D35205F-947E-8343-91A8-87F114B8CE72}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{4993BD12-EFFE-934E-BB6F-C9EA56E54461}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{7995C6AA-4EA8-E344-87A7-877163E13A68}"/>
+    <hyperlink ref="E4" r:id="rId7" xr:uid="{9D595E5E-BDB3-E440-8DE2-044A878B84F4}"/>
+    <hyperlink ref="G5" r:id="rId8" xr:uid="{633A3A15-130A-2B47-83C6-5CABE1D06D19}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{454AAFA7-4F05-1444-A4D1-7702F7578477}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{21CD39D3-F767-4445-96C6-0D6E311D0FEA}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{28FB5FD7-39F3-8043-84AB-B0D588E6AB23}"/>
+    <hyperlink ref="G7" r:id="rId12" xr:uid="{2A55E7CE-60DC-FA4E-99DC-FA00A59F2E76}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2A2828-E136-804F-8DC5-5022B8992DEB}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -655,7 +883,7 @@
     <col min="12" max="16384" width="19.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -666,85 +894,94 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G4" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -756,7 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5AE9F0-A67A-A74A-A726-59E833F8B9AE}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -777,122 +1014,122 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>